<commit_message>
Added score,random gesture functions for RSPRobot, Updated documents for GlovedControl robot
</commit_message>
<xml_diff>
--- a/Project_RPSRobot_20200330_0/Project_RPSRobot_20200330_0.xlsx
+++ b/Project_RPSRobot_20200330_0/Project_RPSRobot_20200330_0.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a59c1bdb761853cd/NAER/EELAB/EELAB/Project_RPSRobot_20200330_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="436" documentId="11_F25DC773A252ABDACC1048E0995B61245BDE58ED" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2655D019-17C8-415D-86B6-63CC950CC079}"/>
+  <xr:revisionPtr revIDLastSave="575" documentId="11_F25DC773A252ABDACC1048E0995B61245BDE58ED" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{58116A87-7C67-4073-9B0C-894CEFDAEF07}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8172" yWindow="372" windowWidth="13992" windowHeight="12084" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HWSystemDiagram" sheetId="1" r:id="rId1"/>
     <sheet name="pins" sheetId="2" r:id="rId2"/>
     <sheet name="ServoDirection" sheetId="3" r:id="rId3"/>
     <sheet name="ServoAdapter" sheetId="4" r:id="rId4"/>
+    <sheet name="工作表1" sheetId="5" r:id="rId5"/>
+    <sheet name="matchScoreTable" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="113">
   <si>
     <t>AVR</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -379,10 +381,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FlexSensors Adapter-Finger4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>UI Board-StartButton</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -455,6 +453,42 @@
   </si>
   <si>
     <t>UI Board-LossLED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Used for Random Seed </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Human</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Robot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -462,7 +496,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,6 +508,14 @@
       <sz val="9"/>
       <name val="新細明體"/>
       <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -546,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -564,6 +606,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -6874,6 +6917,1111 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="直線接點 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{541AE1BF-C0AE-4DF7-B7F0-CBFAF11DE62B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1638300" y="1318260"/>
+          <a:ext cx="7620" cy="4206240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="762901" cy="468013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="文字方塊 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90EBD69A-2A2F-4A60-AE5A-CDCDAA1F1508}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1021080" y="579120"/>
+          <a:ext cx="762901" cy="468013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="2400"/>
+            <a:t>User</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1408655" cy="468013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="文字方塊 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74117B39-7B4A-45CA-AD83-4E7EC3497FD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4320540" y="617220"/>
+          <a:ext cx="1408655" cy="468013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="2400"/>
+            <a:t>RSPRobot</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="2400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="直線單箭頭接點 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A54740C9-3990-49F8-A2A1-45BDDAB9EC85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1653540" y="1897380"/>
+          <a:ext cx="3268980" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1350626" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="文字方塊 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8A8A0B7-2588-4742-B4CA-B83A94829156}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2667000" y="1630680"/>
+          <a:ext cx="1350626" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>Pushs "start" button</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1320361" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="文字方塊 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2E2A613-7602-4187-A7E8-B8E9B113BFED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4259580" y="1996440"/>
+          <a:ext cx="1320361" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>Display</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+            <a:t> countdowm</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1304075" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="文字方塊 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA053CCB-DB82-4247-A3F0-ADC3474D3945}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4282440" y="2948940"/>
+          <a:ext cx="1304075" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>Competition Period</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="右大括弧 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24656E1C-8067-4A35-92B8-080A4896D2CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5509260" y="2788920"/>
+          <a:ext cx="342900" cy="586740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="580095" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="文字方塊 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3DFE8AB-31A0-433B-8490-3EB508E9EACD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5669280" y="2834640"/>
+          <a:ext cx="580095" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+            <a:t>0.5 sec</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-TW" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1354217" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="文字方塊 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6170F81-AC46-4B49-8532-1D5D1CBE0972}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4160520" y="3459480"/>
+          <a:ext cx="1354217" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>Check User Respose</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>(Glove</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+            <a:t> data reading)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-TW" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="639791" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="文字方塊 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18773B6F-20B8-4A2E-87E6-C8377FAB1732}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1333500" y="2979420"/>
+          <a:ext cx="639791" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>Gesture</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="直線單箭頭接點 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47FCFE01-FCAB-4CA6-AA6F-9BC6F946EC59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1661160" y="3238500"/>
+          <a:ext cx="3154680" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="639791" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="文字方塊 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D726F1E4-CB5C-4F77-9721-D72309541ECE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1363980" y="3421380"/>
+          <a:ext cx="639791" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>Keep </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>Gesture</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1296252" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="文字方塊 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CDABD8B-C3BB-4C4F-80AC-9647D253D587}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4290060" y="4229100"/>
+          <a:ext cx="1296252" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>Compute the result</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1180580" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="文字方塊 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15976F96-C19E-409B-938C-BFC1B7A7B80A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4320540" y="4777740"/>
+          <a:ext cx="1180580" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>Display</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100" baseline="0"/>
+            <a:t> the result</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-TW" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="直線接點 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4F6EFAC-7CC9-469B-8291-3F7667018BF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1394460" y="2766060"/>
+          <a:ext cx="4381500" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="直線接點 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7B6C9BC-CAC3-4304-A08B-4E7531E11069}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1424940" y="3406140"/>
+          <a:ext cx="4381500" cy="7620"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="直線接點 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28CE240D-B77A-460D-9FA1-A53A31B47A79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4922520" y="1249680"/>
+          <a:ext cx="7620" cy="4206240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="922945" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name="文字方塊 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3798A79F-CF20-45FC-A893-7996F0A7425C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4511040" y="2392680"/>
+          <a:ext cx="922945" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100"/>
+            <a:t>Servos Move</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7142,7 +8290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="AJ26" sqref="AJ26"/>
     </sheetView>
   </sheetViews>
@@ -7160,7 +8308,7 @@
   <dimension ref="A5:H25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -7219,7 +8367,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>17</v>
@@ -7241,7 +8389,7 @@
         <v>66</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -7265,7 +8413,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>17</v>
@@ -7289,7 +8437,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>39</v>
@@ -7311,7 +8459,7 @@
         <v>69</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>21</v>
@@ -7416,8 +8564,8 @@
       <c r="B16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>85</v>
+      <c r="C16" s="13" t="s">
+        <v>104</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>48</v>
@@ -7440,7 +8588,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>44</v>
@@ -7497,7 +8645,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>27</v>
@@ -7518,7 +8666,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>23</v>
@@ -7541,7 +8689,7 @@
         <v>76</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>37</v>
@@ -7561,7 +8709,7 @@
         <v>77</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>17</v>
@@ -7583,7 +8731,7 @@
         <v>78</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>17</v>
@@ -7605,7 +8753,7 @@
         <v>79</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>42</v>
@@ -7639,35 +8787,35 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" t="s">
         <v>98</v>
-      </c>
-      <c r="C3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" t="s">
         <v>100</v>
-      </c>
-      <c r="C4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
         <v>98</v>
-      </c>
-      <c r="C5" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -7697,4 +8845,139 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7401B850-25D7-4E26-9E19-C6A0AEE4577A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A6A08F1-6316-477B-BE74-D1F207CF513E}">
+  <dimension ref="A4:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added LED driver,Segdisplay driver, integration test for RSPRobot FW. Added EELAB Module_20200404_0
</commit_message>
<xml_diff>
--- a/Project_RPSRobot_20200330_0/Project_RPSRobot_20200330_0.xlsx
+++ b/Project_RPSRobot_20200330_0/Project_RPSRobot_20200330_0.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a59c1bdb761853cd/NAER/EELAB/EELAB/Project_RPSRobot_20200330_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="575" documentId="11_F25DC773A252ABDACC1048E0995B61245BDE58ED" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{58116A87-7C67-4073-9B0C-894CEFDAEF07}"/>
+  <xr:revisionPtr revIDLastSave="588" documentId="11_F25DC773A252ABDACC1048E0995B61245BDE58ED" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6B75B555-81E6-4FCD-9968-278093374913}"/>
   <bookViews>
-    <workbookView xWindow="8172" yWindow="372" windowWidth="13992" windowHeight="12084" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="HWSystemDiagram" sheetId="1" r:id="rId1"/>
-    <sheet name="pins" sheetId="2" r:id="rId2"/>
-    <sheet name="ServoDirection" sheetId="3" r:id="rId3"/>
-    <sheet name="ServoAdapter" sheetId="4" r:id="rId4"/>
-    <sheet name="工作表1" sheetId="5" r:id="rId5"/>
-    <sheet name="matchScoreTable" sheetId="6" r:id="rId6"/>
+    <sheet name="History" sheetId="7" r:id="rId1"/>
+    <sheet name="HWSystemDiagram" sheetId="1" r:id="rId2"/>
+    <sheet name="pins" sheetId="2" r:id="rId3"/>
+    <sheet name="ServoDirection" sheetId="3" r:id="rId4"/>
+    <sheet name="ServoAdapter" sheetId="4" r:id="rId5"/>
+    <sheet name="Interactive sequnce" sheetId="5" r:id="rId6"/>
+    <sheet name="matchScoreTable" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="118">
   <si>
     <t>AVR</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -489,6 +490,27 @@
   </si>
   <si>
     <t>W</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Win</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lose</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added sheet "matchScoreTable"
+Modified sheet "pins"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NAER T.I.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -588,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -607,6 +629,9 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -8287,6 +8312,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC3886C-F60B-4A5C-A85A-A3DB892384B4}">
+  <dimension ref="A4:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>20200404</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -8303,7 +8360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD0389E1-4AFF-475A-90D0-EB65AF0D5B90}">
   <dimension ref="A5:H25"/>
   <sheetViews>
@@ -8772,7 +8829,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B20BD5A-8D8A-4622-8FF4-009BC882D92D}">
   <dimension ref="A3:C5"/>
   <sheetViews>
@@ -8826,7 +8883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2F1A10-2D19-4BB8-A7AC-162D371FEE94}">
   <dimension ref="O5"/>
   <sheetViews>
@@ -8847,12 +8904,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7401B850-25D7-4E26-9E19-C6A0AEE4577A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -8863,12 +8920,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A6A08F1-6316-477B-BE74-D1F207CF513E}">
   <dimension ref="A4:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -8954,7 +9011,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -8962,7 +9019,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -8970,7 +9027,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -8979,5 +9036,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed issue #2 "the object box does not be displayed on the live window"
</commit_message>
<xml_diff>
--- a/Project_RPSRobot_20200330_0/Project_RPSRobot_20200330_0.xlsx
+++ b/Project_RPSRobot_20200330_0/Project_RPSRobot_20200330_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a59c1bdb761853cd/NAER/EELAB/EELAB/Project_RPSRobot_20200330_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="114_{BAB8388F-520A-4786-92C7-6169383AA95C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6CB9B44C-D679-4C7B-8D17-46003CCF3A44}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="114_{BAB8388F-520A-4786-92C7-6169383AA95C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EAA478F1-1D2A-4385-8AA5-A5ECE639E54A}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="8520" yWindow="276" windowWidth="12504" windowHeight="12084" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="History" sheetId="7" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="MachineLearningANN_2" sheetId="11" r:id="rId9"/>
     <sheet name="工作表1" sheetId="9" r:id="rId10"/>
     <sheet name="scoreBoard" sheetId="10" r:id="rId11"/>
+    <sheet name="Overview" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23545,6 +23546,72 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="圖片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{304A6E42-7B1B-4499-90C6-1D49DE92842A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10721340" cy="6256020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -23808,10 +23875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC3886C-F60B-4A5C-A85A-A3DB892384B4}">
-  <dimension ref="A4:C10"/>
+  <dimension ref="A4:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -23881,6 +23948,9 @@
       <c r="B10" s="14" t="s">
         <v>131</v>
       </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -24054,8 +24124,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A1B622-AE3F-452A-B88F-5E455B497A82}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393B70F7-CE77-43E8-8948-5F4091DCCBCF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -27684,7 +27771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBCFBDB-5166-480F-80AB-8FD60A7D3C4C}">
   <dimension ref="E3:AY62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AF12" sqref="AF12:AY42"/>
     </sheetView>
   </sheetViews>

</xml_diff>